<commit_message>
📊 Atualiza layout de gráficos e corrige indentação final
</commit_message>
<xml_diff>
--- a/data/logs/log_classificacoes.xlsx
+++ b/data/logs/log_classificacoes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D171"/>
+  <dimension ref="A1:D267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3515,6 +3515,1734 @@
         </is>
       </c>
     </row>
+    <row r="172">
+      <c r="A172" t="inlineStr"/>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr"/>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr"/>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr"/>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr"/>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr"/>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr"/>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr"/>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr"/>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr"/>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr"/>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr"/>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:02:09</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr"/>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr"/>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr"/>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr"/>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr"/>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr"/>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr"/>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr"/>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr"/>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr"/>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr"/>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr"/>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:10:25</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr"/>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr"/>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr"/>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr"/>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr"/>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr"/>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr"/>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr"/>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr"/>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr"/>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr"/>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr"/>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:21:10</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr"/>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr"/>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr"/>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr"/>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr"/>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr"/>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr"/>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr"/>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr"/>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr"/>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr"/>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr"/>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:33:04</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr"/>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr"/>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr"/>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr"/>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr"/>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr"/>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr"/>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr"/>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr"/>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr"/>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr"/>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr"/>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:44:02</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr"/>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr"/>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr"/>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr"/>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr"/>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr"/>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr"/>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr"/>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr"/>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr"/>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr"/>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr"/>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:55:09</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr"/>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr"/>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr"/>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr"/>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr"/>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr"/>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr"/>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr"/>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr"/>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr"/>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr"/>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr"/>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:00:58</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr"/>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>SEM SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr"/>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>TV</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>MANCHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr"/>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>RISCADO</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr"/>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>AWS</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>QUEDA</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr"/>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>FGH</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>SOM ALTO</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr"/>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>NÃO LIGA</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr"/>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>ASD</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>NÃO DA SOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr"/>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>HFG</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>SEM AUDIO</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr"/>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>TJND</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>SEM SINAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr"/>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr"/>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>NFGH</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>SEM BOBINA</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr"/>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>BBS</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>2025-11-06 16:04:26</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>SEM LED</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>